<commit_message>
30/10/24-DuyLVD Update Create question import file
</commit_message>
<xml_diff>
--- a/public/TemplateCreateQuestion.xlsx
+++ b/public/TemplateCreateQuestion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duylv\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D3A132-FDA0-4E37-8FF1-C716283F876F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872B2963-0B21-4779-894B-41E284895E22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{0FF3ECD7-9910-4479-A43B-32283162E1F9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="42">
   <si>
     <t>Content</t>
   </si>
@@ -135,23 +135,29 @@
     <t>isCorrectAnswer</t>
   </si>
   <si>
-    <t>Label</t>
-  </si>
-  <si>
-    <t>Text</t>
-  </si>
-  <si>
     <t>A (Math)</t>
   </si>
   <si>
     <t>B (Reading &amp; Writing)</t>
+  </si>
+  <si>
+    <t>Answer 1</t>
+  </si>
+  <si>
+    <t>Answer 2</t>
+  </si>
+  <si>
+    <t>Answer 3</t>
+  </si>
+  <si>
+    <t>Answer 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,6 +288,34 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF1B212F"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -634,7 +668,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -642,14 +676,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1031,151 +1071,162 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A69A577-1844-4376-B71C-1EE850C684F6}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="77.875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="55.25" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.125" style="2" customWidth="1"/>
     <col min="3" max="3" width="12.5" style="2" customWidth="1"/>
     <col min="4" max="4" width="22.75" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35.25" style="2" customWidth="1"/>
     <col min="6" max="6" width="23.75" style="2" customWidth="1"/>
     <col min="7" max="7" width="16.625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="8.875" style="2"/>
-    <col min="9" max="9" width="34.625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="31.25" style="2" customWidth="1"/>
+    <col min="9" max="9" width="19.125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="21.25" style="2" customWidth="1"/>
+    <col min="11" max="11" width="18.5" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="H1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="5"/>
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="5"/>
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="5"/>
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="5"/>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="5"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="5"/>
-    </row>
-    <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="5"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="5"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="5"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
     </row>
     <row r="17" spans="3:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
@@ -1207,20 +1258,18 @@
       <c r="G22" s="1"/>
     </row>
   </sheetData>
-  <dataValidations count="6">
+  <phoneticPr fontId="21" type="noConversion"/>
+  <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C21" xr:uid="{A4987C9D-7827-47CD-81C6-D9701D73D676}">
       <formula1>"Foundation,Medium,Advance"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E575" xr:uid="{29724948-C531-485D-B224-3143C206D1E9}">
       <formula1>$A$578:$A$606</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1" xr:uid="{6ECA5CC2-BB62-49B6-B598-FC923C6B73A9}">
-      <formula1>"Area and volume;Lines, angles, and triangles"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G22" xr:uid="{8A61253D-0C06-492C-BCA5-6E6DFD18D2EE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G17:G22 F2:F22" xr:uid="{8A61253D-0C06-492C-BCA5-6E6DFD18D2EE}">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E5" xr:uid="{1598EBE5-DD3D-460C-8349-2454260520FD}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E9" xr:uid="{1598EBE5-DD3D-460C-8349-2454260520FD}">
       <formula1>INDIRECT($D$2)</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D22" xr:uid="{2BF4742F-EA8A-4296-85EA-3BC05C0D6D06}">
@@ -1236,7 +1285,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$A$1:$A$29</xm:f>
           </x14:formula1>
-          <xm:sqref>E6:E22</xm:sqref>
+          <xm:sqref>E10:E22</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1266,11 +1315,11 @@
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>39</v>
+      <c r="J2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>